<commit_message>
Memperbarui berkas data sampel-presensi
</commit_message>
<xml_diff>
--- a/data/sampel-presensi.xlsx
+++ b/data/sampel-presensi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\SGS\17. Program\Python\laporan-presensi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\SGS\17. Program\Python\analisis-data-administrasi-akademik\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4AC72B-B358-4CB7-9C17-DC88A4D90F8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF1CE1B-0CA6-4684-A209-2CD173E6FC57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5385" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1696" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1792" uniqueCount="172">
   <si>
     <t>Presensi Perkuliahan Mahasiswa Tahun Ajaran 2020/2021 Semester Gasal</t>
   </si>
@@ -536,12 +536,45 @@
   <si>
     <t>91K2101 - Mata Kuliah A</t>
   </si>
+  <si>
+    <t>Mahasiswa 7</t>
+  </si>
+  <si>
+    <t>91S18015</t>
+  </si>
+  <si>
+    <t>Mahasiswa 8</t>
+  </si>
+  <si>
+    <t>Mahasiswa 9</t>
+  </si>
+  <si>
+    <t>91S18017</t>
+  </si>
+  <si>
+    <t>Mahasiswa 10</t>
+  </si>
+  <si>
+    <t>91S18018</t>
+  </si>
+  <si>
+    <t>Mahasiswa 11</t>
+  </si>
+  <si>
+    <t>91S18019</t>
+  </si>
+  <si>
+    <t>Mahasiswa 12</t>
+  </si>
+  <si>
+    <t>91S18020</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -568,6 +601,10 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -825,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S975"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1367,12 +1404,342 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C25" s="3">
+        <v>13</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S25" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C26" s="3">
+        <v>13</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S26" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C27" s="3">
+        <v>13</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S27" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C28" s="3">
+        <v>13</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S28" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C29" s="3">
+        <v>13</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S29" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C30" s="3">
+        <v>11</v>
+      </c>
+      <c r="D30" s="3">
+        <v>2</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S30" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="31" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2319,6 +2686,7 @@
     <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>